<commit_message>
changes on the codeblock of the function
</commit_message>
<xml_diff>
--- a/assets/Sources(AutoRecovered).xlsx
+++ b/assets/Sources(AutoRecovered).xlsx
@@ -1159,8 +1159,8 @@
   </sheetPr>
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F74" activeCellId="0" sqref="F74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E77" activeCellId="0" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="H4" s="12" t="n">
         <f aca="false">COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H5" s="14" t="n">
         <f aca="false">COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2284,7 @@
         <v>162</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixed the new fucntion
</commit_message>
<xml_diff>
--- a/assets/Sources(AutoRecovered).xlsx
+++ b/assets/Sources(AutoRecovered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAFD362-B897-4573-BEA4-9098EDD2CAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCDBB5E-582B-4CC4-B5F4-D43B503B01DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1133,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="H4" s="11">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="H5" s="13">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
         <v>164</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished a new function
</commit_message>
<xml_diff>
--- a/assets/Sources(AutoRecovered).xlsx
+++ b/assets/Sources(AutoRecovered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCDBB5E-582B-4CC4-B5F4-D43B503B01DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288D5E2D-D14A-4096-8F7B-057C9D18B56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1133,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="H4" s="11">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="H5" s="13">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1484,7 +1484,7 @@
       <c r="B22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -2366,11 +2366,11 @@
       <c r="B85" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="16" t="s">
         <v>178</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>180</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,7 +2394,7 @@
       <c r="B87" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="16" t="s">
         <v>182</v>
       </c>
       <c r="D87" s="2" t="s">

</xml_diff>